<commit_message>
added the largest rectangle in the histogram code, but it seem to not work for all the test cases, need to modify in the future. NOT the best code, just the bruteforce approach
</commit_message>
<xml_diff>
--- a/Important-450-DSA.xlsx
+++ b/Important-450-DSA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piyush\Desktop\90DaysOfDSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916E1AE6-15C7-495D-B157-86917B895A4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4BC2409-3442-46FB-A5BE-8D9A284A4CE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1504,7 +1504,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1514,6 +1514,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1531,7 +1537,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1559,6 +1565,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1878,8 +1887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A452" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B409" sqref="B409"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6175,8 +6184,8 @@
       <c r="B410" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="C410" s="2" t="s">
-        <v>3</v>
+      <c r="C410" s="13" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="411" spans="1:3" ht="21">
@@ -6186,8 +6195,8 @@
       <c r="B411" s="4" t="s">
         <v>394</v>
       </c>
-      <c r="C411" s="2" t="s">
-        <v>3</v>
+      <c r="C411" s="13" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="412" spans="1:3" ht="21">

</xml_diff>